<commit_message>
dfm3 for states done
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vs_code\python\AI_DA_DFM-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C1BAA5-06F6-44E3-A6CF-4DE9B0DA25A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70637E8-CBA5-45A6-9AF1-B4B4C0F5C43D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>con_string_mis_warehouse</t>
   </si>
@@ -67,6 +67,60 @@
   </si>
   <si>
     <t>weather database connection string</t>
+  </si>
+  <si>
+    <t>holidayExcelPath</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0047000</t>
+  </si>
+  <si>
+    <t>WR virtual weather station name</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046980</t>
+  </si>
+  <si>
+    <t>mah virtual weather station name</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046957</t>
+  </si>
+  <si>
+    <t>Gujarat  virtual weather station name</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046978</t>
+  </si>
+  <si>
+    <t>MP  virtual weather station name</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046945</t>
+  </si>
+  <si>
+    <t>Chatt  virtual weather station name</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046962</t>
+  </si>
+  <si>
+    <t>Goa  virtual weather station name</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046948</t>
+  </si>
+  <si>
+    <t>DD  virtual weather station name</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046953</t>
+  </si>
+  <si>
+    <t>DNH  virtual weather station name</t>
+  </si>
+  <si>
+    <t>holiday excel folder path</t>
   </si>
 </sst>
 </file>
@@ -404,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,6 +526,78 @@
         <v>13</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="mis_warehouse/wrldc#123@10.2.100.56:15210/ORCLWR" xr:uid="{98848ACB-4C2A-4A35-A1C8-AEC84B89C8E8}"/>

</xml_diff>